<commit_message>
Update CK SP Default version
</commit_message>
<xml_diff>
--- a/002-‘’Choco‘’SpecialRemake/003-PickAndPlace_Special_remake.xlsx
+++ b/002-‘’Choco‘’SpecialRemake/003-PickAndPlace_Special_remake.xlsx
@@ -1,17 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6855E2EA-233D-4A57-B8BB-2E6984FC1BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="2790" yWindow="1940" windowWidth="14970" windowHeight="13030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="PickAndPlace_Special remake_202" state="visible" r:id="rId4"/>
+    <sheet name="PickAndPlace_Special remake_2_2" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="129">
   <si>
     <t>Designator</t>
   </si>
@@ -151,320 +155,273 @@
     <t>6.486mm</t>
   </si>
   <si>
-    <t>BAT</t>
-  </si>
-  <si>
-    <t>HDR-M-2.54_1x2</t>
-  </si>
-  <si>
-    <t>HDR-M-2.54_1X2</t>
-  </si>
-  <si>
-    <t>3.81mm</t>
-  </si>
-  <si>
-    <t>-47.625mm</t>
-  </si>
-  <si>
-    <t>2.54mm</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
-    <t>UART</t>
-  </si>
-  <si>
-    <t>CH340K</t>
-  </si>
-  <si>
-    <t>ESOP-10_L4.9-W3.9-P1.00-LS6.2-BL-EP</t>
+    <t>USB</t>
+  </si>
+  <si>
+    <t>TYPE-C 16PIN 2MD(073)</t>
+  </si>
+  <si>
+    <t>USB-C-SMD_TYPE-C-6PIN-2MD-073</t>
+  </si>
+  <si>
+    <t>15mm</t>
+  </si>
+  <si>
+    <t>18.2mm</t>
+  </si>
+  <si>
+    <t>-7.201mm</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>180kΩ</t>
+  </si>
+  <si>
+    <t>28.956mm</t>
+  </si>
+  <si>
+    <t>-10.16mm</t>
+  </si>
+  <si>
+    <t>-10.913mm</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>100nF</t>
+  </si>
+  <si>
+    <t>14.605mm</t>
+  </si>
+  <si>
+    <t>15.305mm</t>
+  </si>
+  <si>
+    <t>RD2</t>
+  </si>
+  <si>
+    <t>5.1kΩ</t>
+  </si>
+  <si>
+    <t>-3.175mm</t>
+  </si>
+  <si>
+    <t>RD1</t>
+  </si>
+  <si>
+    <t>-1.524mm</t>
+  </si>
+  <si>
+    <t>RD</t>
+  </si>
+  <si>
+    <t>4.7kΩ</t>
+  </si>
+  <si>
+    <t>17.78mm</t>
+  </si>
+  <si>
+    <t>18.533mm</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>24.003mm</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>22.098mm</t>
+  </si>
+  <si>
+    <t>-9.398mm</t>
+  </si>
+  <si>
+    <t>-10.151mm</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>20.193mm</t>
+  </si>
+  <si>
+    <t>SW</t>
+  </si>
+  <si>
+    <t>SSSS811101</t>
+  </si>
+  <si>
+    <t>SW-SMD_SSSS811101</t>
+  </si>
+  <si>
+    <t>2.286mm</t>
+  </si>
+  <si>
+    <t>-16.002mm</t>
+  </si>
+  <si>
+    <t>3.836mm</t>
+  </si>
+  <si>
+    <t>-13.752mm</t>
+  </si>
+  <si>
+    <t>VD1</t>
+  </si>
+  <si>
+    <t>220kΩ</t>
+  </si>
+  <si>
+    <t>27.305mm</t>
+  </si>
+  <si>
+    <t>-9.407mm</t>
+  </si>
+  <si>
+    <t>VD2</t>
+  </si>
+  <si>
+    <t>100kΩ</t>
+  </si>
+  <si>
+    <t>25.654mm</t>
+  </si>
+  <si>
+    <t>LDO3V3</t>
+  </si>
+  <si>
+    <t>ME6211C33M5G-N</t>
+  </si>
+  <si>
+    <t>SOT-23-5_L3.0-W1.7-P0.95-LS2.8-BL</t>
+  </si>
+  <si>
+    <t>-22.733mm</t>
+  </si>
+  <si>
+    <t>1.64mm</t>
+  </si>
+  <si>
+    <t>-21.783mm</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>TP4057-42-SOT26-R</t>
+  </si>
+  <si>
+    <t>SOT-23-6_L2.9-W1.6-P0.95-LS2.8-BL</t>
+  </si>
+  <si>
+    <t>-9.271mm</t>
+  </si>
+  <si>
+    <t>6.09mm</t>
+  </si>
+  <si>
+    <t>-8.321mm</t>
+  </si>
+  <si>
+    <t>ESP1</t>
+  </si>
+  <si>
+    <t>ESP-12F(ESP8266MOD)</t>
+  </si>
+  <si>
+    <t>WIFIM-SMD_ESP-12F-ESP8266MOD</t>
+  </si>
+  <si>
+    <t>14.113mm</t>
+  </si>
+  <si>
+    <t>-19.712mm</t>
+  </si>
+  <si>
+    <t>13.462mm</t>
+  </si>
+  <si>
+    <t>21.113mm</t>
+  </si>
+  <si>
+    <t>-12.161mm</t>
+  </si>
+  <si>
+    <t>2.4GHz</t>
+  </si>
+  <si>
+    <t>UART1</t>
+  </si>
+  <si>
+    <t>CH340X</t>
+  </si>
+  <si>
+    <t>MSOP-10_L3.0-W3.0-P0.50-LS5.0-BL</t>
+  </si>
+  <si>
+    <t>24.867mm</t>
+  </si>
+  <si>
+    <t>-4.699mm</t>
+  </si>
+  <si>
+    <t>22.757mm</t>
+  </si>
+  <si>
+    <t>-3.699mm</t>
+  </si>
+  <si>
+    <t>R10</t>
   </si>
   <si>
     <t>24.892mm</t>
   </si>
   <si>
-    <t>-3.429mm</t>
-  </si>
-  <si>
-    <t>22.142mm</t>
-  </si>
-  <si>
-    <t>-1.429mm</t>
-  </si>
-  <si>
-    <t>USB</t>
-  </si>
-  <si>
-    <t>TYPE-C 16PIN 2MD(073)</t>
-  </si>
-  <si>
-    <t>USB-C-SMD_TYPE-C-6PIN-2MD-073</t>
-  </si>
-  <si>
-    <t>15mm</t>
-  </si>
-  <si>
-    <t>-4.572mm</t>
-  </si>
-  <si>
-    <t>18.2mm</t>
-  </si>
-  <si>
-    <t>-6.947mm</t>
-  </si>
-  <si>
-    <t>RS</t>
-  </si>
-  <si>
-    <t>180kΩ</t>
-  </si>
-  <si>
-    <t>28.956mm</t>
-  </si>
-  <si>
-    <t>-10.16mm</t>
-  </si>
-  <si>
-    <t>-10.913mm</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>100nF</t>
-  </si>
-  <si>
-    <t>14.605mm</t>
-  </si>
-  <si>
-    <t>15.305mm</t>
-  </si>
-  <si>
-    <t>RD2</t>
-  </si>
-  <si>
-    <t>5.1kΩ</t>
-  </si>
-  <si>
-    <t>-3.175mm</t>
-  </si>
-  <si>
-    <t>RD1</t>
-  </si>
-  <si>
-    <t>-1.524mm</t>
-  </si>
-  <si>
-    <t>RD</t>
-  </si>
-  <si>
-    <t>4.7kΩ</t>
-  </si>
-  <si>
-    <t>17.78mm</t>
-  </si>
-  <si>
-    <t>18.533mm</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>24.003mm</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>22.098mm</t>
-  </si>
-  <si>
-    <t>-9.398mm</t>
-  </si>
-  <si>
-    <t>-10.151mm</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>20.193mm</t>
-  </si>
-  <si>
-    <t>SW</t>
-  </si>
-  <si>
-    <t>SSSS811101</t>
-  </si>
-  <si>
-    <t>SW-SMD_SSSS811101</t>
-  </si>
-  <si>
-    <t>2.159mm</t>
-  </si>
-  <si>
-    <t>-16mm</t>
-  </si>
-  <si>
-    <t>3.709mm</t>
-  </si>
-  <si>
-    <t>-13.75mm</t>
-  </si>
-  <si>
-    <t>VD1</t>
-  </si>
-  <si>
-    <t>220kΩ</t>
-  </si>
-  <si>
-    <t>27.305mm</t>
-  </si>
-  <si>
-    <t>-9.407mm</t>
-  </si>
-  <si>
-    <t>VD2</t>
-  </si>
-  <si>
-    <t>100kΩ</t>
-  </si>
-  <si>
-    <t>25.654mm</t>
-  </si>
-  <si>
-    <t>LDO3V3</t>
-  </si>
-  <si>
-    <t>ME6211C33M5G-N</t>
-  </si>
-  <si>
-    <t>SOT-23-5_L3.0-W1.7-P0.95-LS2.8-BL</t>
-  </si>
-  <si>
-    <t>-22.733mm</t>
-  </si>
-  <si>
-    <t>1.64mm</t>
-  </si>
-  <si>
-    <t>-21.783mm</t>
-  </si>
-  <si>
-    <t>P1</t>
-  </si>
-  <si>
-    <t>TP4057-42-SOT26-R</t>
-  </si>
-  <si>
-    <t>SOT-23-6_L2.9-W1.6-P0.95-LS2.8-BL</t>
-  </si>
-  <si>
-    <t>-9.271mm</t>
-  </si>
-  <si>
-    <t>6.09mm</t>
-  </si>
-  <si>
-    <t>-8.321mm</t>
-  </si>
-  <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>UMH3N</t>
-  </si>
-  <si>
-    <t>SC-70-6_L2.2-W1.3-P0.65-LS2.1-BR</t>
-  </si>
-  <si>
-    <t>-7.366mm</t>
-  </si>
-  <si>
-    <t>25.842mm</t>
-  </si>
-  <si>
-    <t>-8.016mm</t>
-  </si>
-  <si>
-    <t>CONN1</t>
-  </si>
-  <si>
-    <t>HDR-M_2.54_1x10P</t>
-  </si>
-  <si>
-    <t>HDR-TH_10P-P2.54-V-M-1</t>
-  </si>
-  <si>
-    <t>14.986mm</t>
-  </si>
-  <si>
-    <t>-43.307mm</t>
-  </si>
-  <si>
-    <t>3.556mm</t>
-  </si>
-  <si>
-    <t>J1</t>
-  </si>
-  <si>
-    <t>POGO-F-2.5_1x2</t>
-  </si>
-  <si>
-    <t>POGO-F-2pin-2.5mm</t>
-  </si>
-  <si>
-    <t>-47.564mm</t>
-  </si>
-  <si>
-    <t>-49.276mm</t>
-  </si>
-  <si>
-    <t>16.25mm</t>
-  </si>
-  <si>
-    <t>ESP1</t>
-  </si>
-  <si>
-    <t>ESP-12F(ESP8266MOD)</t>
-  </si>
-  <si>
-    <t>WIFIM-SMD_ESP-12F-ESP8266MOD</t>
-  </si>
-  <si>
-    <t>14.209mm</t>
-  </si>
-  <si>
-    <t>-20.008mm</t>
-  </si>
-  <si>
-    <t>13.558mm</t>
-  </si>
-  <si>
-    <t>21.209mm</t>
-  </si>
-  <si>
-    <t>-12.457mm</t>
-  </si>
-  <si>
-    <t>2.4GHz</t>
+    <t>-7.62mm</t>
+  </si>
+  <si>
+    <t>24.139mm</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>CC0603KRX7R9BB104</t>
+  </si>
+  <si>
+    <t>28.067mm</t>
+  </si>
+  <si>
+    <t>27.367mm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -491,7 +448,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -827,12 +784,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="14" width="20" customWidth="1"/>
   </cols>
@@ -1145,165 +1104,122 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" t="s">
-        <v>49</v>
-      </c>
-      <c r="G8" t="s">
-        <v>50</v>
-      </c>
-      <c r="H8" t="s">
-        <v>51</v>
-      </c>
-      <c r="I8" t="s">
-        <v>50</v>
-      </c>
-      <c r="J8">
-        <v>2</v>
-      </c>
-      <c r="K8" t="s">
-        <v>52</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8" t="s">
-        <v>53</v>
-      </c>
-      <c r="N8" t="s">
-        <v>47</v>
-      </c>
-    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D9" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="E9" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="F9" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="G9" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="H9" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="I9" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="J9">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="K9" t="s">
         <v>20</v>
       </c>
       <c r="L9">
-        <v>-90</v>
+        <v>180</v>
       </c>
       <c r="M9" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="N9" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="E10" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="F10" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="G10" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="H10" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="I10" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="J10">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="K10" t="s">
         <v>20</v>
       </c>
       <c r="L10">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="M10" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="N10" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="E11" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="F11" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="G11" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="H11" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="I11" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="J11">
         <v>2</v>
@@ -1312,42 +1228,42 @@
         <v>20</v>
       </c>
       <c r="L11">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="M11" t="s">
         <v>21</v>
       </c>
       <c r="N11" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B12" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>75</v>
+        <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="F12" t="s">
-        <v>75</v>
+        <v>17</v>
       </c>
       <c r="G12" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="H12" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
       <c r="I12" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="J12">
         <v>2</v>
@@ -1356,21 +1272,21 @@
         <v>20</v>
       </c>
       <c r="L12">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="M12" t="s">
         <v>21</v>
       </c>
       <c r="N12" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="B13" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="C13" t="s">
         <v>16</v>
@@ -1379,19 +1295,19 @@
         <v>17</v>
       </c>
       <c r="E13" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="F13" t="s">
         <v>17</v>
       </c>
       <c r="G13" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="H13" t="s">
         <v>45</v>
       </c>
       <c r="I13" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="J13">
         <v>2</v>
@@ -1406,36 +1322,36 @@
         <v>21</v>
       </c>
       <c r="N13" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="B14" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
       <c r="E14" t="s">
-        <v>81</v>
+        <v>40</v>
       </c>
       <c r="F14" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
       <c r="G14" t="s">
-        <v>81</v>
+        <v>40</v>
       </c>
       <c r="H14" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="I14" t="s">
-        <v>81</v>
+        <v>40</v>
       </c>
       <c r="J14">
         <v>2</v>
@@ -1444,42 +1360,42 @@
         <v>20</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="M14" t="s">
         <v>21</v>
       </c>
       <c r="N14" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="B15" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="C15" t="s">
         <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="E15" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="F15" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="G15" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="H15" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="I15" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="J15">
         <v>2</v>
@@ -1488,42 +1404,42 @@
         <v>20</v>
       </c>
       <c r="L15">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="M15" t="s">
         <v>21</v>
       </c>
       <c r="N15" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="B16" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="C16" t="s">
         <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="E16" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F16" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="G16" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="H16" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="I16" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="J16">
         <v>2</v>
@@ -1538,36 +1454,36 @@
         <v>21</v>
       </c>
       <c r="N16" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B17" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="C17" t="s">
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="E17" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="F17" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="G17" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="H17" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="I17" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="J17">
         <v>2</v>
@@ -1582,83 +1498,83 @@
         <v>21</v>
       </c>
       <c r="N17" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="B18" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" t="s">
+        <v>82</v>
+      </c>
+      <c r="E18" t="s">
         <v>83</v>
       </c>
-      <c r="C18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" t="s">
-        <v>93</v>
-      </c>
-      <c r="E18" t="s">
-        <v>90</v>
-      </c>
       <c r="F18" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="G18" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="H18" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="I18" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="J18">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="K18" t="s">
         <v>20</v>
       </c>
       <c r="L18">
-        <v>90</v>
+        <v>-90</v>
       </c>
       <c r="M18" t="s">
         <v>21</v>
       </c>
       <c r="N18" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B19" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C19" t="s">
-        <v>96</v>
+        <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="E19" t="s">
-        <v>98</v>
+        <v>56</v>
       </c>
       <c r="F19" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="G19" t="s">
-        <v>98</v>
+        <v>56</v>
       </c>
       <c r="H19" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="I19" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="J19">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="K19" t="s">
         <v>20</v>
@@ -1670,36 +1586,36 @@
         <v>21</v>
       </c>
       <c r="N19" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="B20" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="C20" t="s">
         <v>16</v>
       </c>
       <c r="D20" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="E20" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="F20" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="G20" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="H20" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="I20" t="s">
-        <v>104</v>
+        <v>57</v>
       </c>
       <c r="J20">
         <v>2</v>
@@ -1708,262 +1624,219 @@
         <v>20</v>
       </c>
       <c r="L20">
-        <v>270</v>
+        <v>90</v>
       </c>
       <c r="M20" t="s">
         <v>21</v>
       </c>
       <c r="N20" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="B21" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="C21" t="s">
-        <v>16</v>
+        <v>95</v>
       </c>
       <c r="D21" t="s">
-        <v>107</v>
+        <v>32</v>
       </c>
       <c r="E21" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
       <c r="F21" t="s">
-        <v>107</v>
+        <v>32</v>
       </c>
       <c r="G21" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
       <c r="H21" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="I21" t="s">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="J21">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K21" t="s">
         <v>20</v>
       </c>
       <c r="L21">
-        <v>90</v>
+        <v>-90</v>
       </c>
       <c r="M21" t="s">
         <v>21</v>
       </c>
       <c r="N21" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="B22" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C22" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="D22" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="E22" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="F22" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="G22" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="H22" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="I22" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="J22">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K22" t="s">
         <v>20</v>
       </c>
       <c r="L22">
-        <v>270</v>
+        <v>-90</v>
       </c>
       <c r="M22" t="s">
         <v>21</v>
       </c>
       <c r="N22" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>114</v>
-      </c>
-      <c r="B23" t="s">
-        <v>115</v>
-      </c>
-      <c r="C23" t="s">
-        <v>116</v>
-      </c>
-      <c r="D23" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" t="s">
-        <v>117</v>
-      </c>
-      <c r="F23" t="s">
-        <v>17</v>
-      </c>
-      <c r="G23" t="s">
-        <v>117</v>
-      </c>
-      <c r="H23" t="s">
-        <v>118</v>
-      </c>
-      <c r="I23" t="s">
-        <v>119</v>
-      </c>
-      <c r="J23">
-        <v>6</v>
-      </c>
-      <c r="K23" t="s">
-        <v>20</v>
-      </c>
-      <c r="L23">
-        <v>270</v>
-      </c>
-      <c r="M23" t="s">
-        <v>21</v>
-      </c>
-      <c r="N23" t="s">
-        <v>115</v>
-      </c>
-    </row>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="B24" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="C24" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="D24" t="s">
-        <v>57</v>
+        <v>108</v>
       </c>
       <c r="E24" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="F24" t="s">
-        <v>57</v>
+        <v>110</v>
       </c>
       <c r="G24" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="H24" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="I24" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="J24">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="K24" t="s">
         <v>20</v>
       </c>
       <c r="L24">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="M24" t="s">
         <v>21</v>
       </c>
       <c r="N24" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="B25" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="C25" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="D25" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="E25" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="F25" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="G25" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="H25" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="I25" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="J25">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="K25" t="s">
         <v>20</v>
       </c>
       <c r="L25">
-        <v>0</v>
+        <v>-90</v>
       </c>
       <c r="M25" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="N25" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="B26" t="s">
-        <v>133</v>
+        <v>68</v>
       </c>
       <c r="C26" t="s">
-        <v>134</v>
+        <v>16</v>
       </c>
       <c r="D26" t="s">
-        <v>64</v>
+        <v>122</v>
       </c>
       <c r="E26" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="F26" t="s">
-        <v>64</v>
+        <v>122</v>
       </c>
       <c r="G26" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="H26" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="I26" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="J26">
         <v>2</v>
@@ -1972,62 +1845,63 @@
         <v>20</v>
       </c>
       <c r="L26">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="M26" t="s">
         <v>21</v>
       </c>
       <c r="N26" t="s">
-        <v>133</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="B27" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="C27" t="s">
-        <v>140</v>
+        <v>31</v>
       </c>
       <c r="D27" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="E27" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="F27" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="G27" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="H27" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="I27" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="J27">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="K27" t="s">
         <v>20</v>
       </c>
       <c r="L27">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="M27" t="s">
         <v>21</v>
       </c>
       <c r="N27" t="s">
-        <v>146</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>